<commit_message>
Add Response Time upload Excel
</commit_message>
<xml_diff>
--- a/td_toolkits_v3/opticals/tests/test_files/test_2/Chips Upload.xlsx
+++ b/td_toolkits_v3/opticals/tests/test_files/test_2/Chips Upload.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\實驗\Projects\寬溫LC\RD Line\5905\光學\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dimsp\Documents\Projects\td_toolkits_v3\td_toolkits_v3\opticals\tests\test_files\test_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093F3124-9EE0-4BFB-BCC0-FA32B9DEFCE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="1"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="registerted" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="319">
   <si>
     <t>item</t>
   </si>
@@ -189,13 +190,6 @@
   </si>
   <si>
     <t>1-22</t>
-  </si>
-  <si>
-    <t>RD11104010</t>
-  </si>
-  <si>
-    <t>RD11104010</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>寬溫負型液晶</t>
@@ -681,10 +675,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>RD11104009</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>T108C001NV25</t>
   </si>
   <si>
@@ -1019,12 +1009,16 @@
   </si>
   <si>
     <t>1F-15</t>
+  </si>
+  <si>
+    <t>RD11104009+RD11104010</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1413,7 +1407,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1435,7 +1429,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1451,7 +1445,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1467,7 +1461,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1507,7 +1501,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1741,17 +1735,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J120"/>
+      <selection activeCell="B2" sqref="B2:B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -1797,25 +1791,25 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C2" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>7</v>
@@ -1829,25 +1823,25 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C3" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="F3" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>7</v>
@@ -1861,25 +1855,25 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C4" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>7</v>
@@ -1893,25 +1887,25 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C5" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>7</v>
@@ -1925,25 +1919,25 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C6" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>7</v>
@@ -1957,25 +1951,25 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C7" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>7</v>
@@ -1989,25 +1983,25 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C8" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="F8" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>7</v>
@@ -2021,25 +2015,25 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C9" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="F9" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>7</v>
@@ -2053,25 +2047,25 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C10" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="F10" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>7</v>
@@ -2085,25 +2079,25 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C11" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="E11" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>7</v>
@@ -2117,25 +2111,25 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C12" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="E12" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>7</v>
@@ -2149,25 +2143,25 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C13" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="E13" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>7</v>
@@ -2181,25 +2175,25 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C14" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="E14" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="G14" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>12</v>
@@ -2213,25 +2207,25 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C15" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="E15" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>12</v>
@@ -2245,25 +2239,25 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C16" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="E16" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>12</v>
@@ -2277,25 +2271,25 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C17" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="E17" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>12</v>
@@ -2309,25 +2303,25 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C18" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="E18" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>12</v>
@@ -2341,25 +2335,25 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C19" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="E19" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>12</v>
@@ -2373,25 +2367,25 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C20" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="E20" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>12</v>
@@ -2405,25 +2399,25 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C21" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="E21" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>12</v>
@@ -2437,25 +2431,25 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C22" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="E22" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>12</v>
@@ -2469,25 +2463,25 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C23" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E23" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>5</v>
@@ -2501,25 +2495,25 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C24" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E24" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>5</v>
@@ -2533,25 +2527,25 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C25" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E25" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>5</v>
@@ -2565,25 +2559,25 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C26" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E26" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>5</v>
@@ -2597,25 +2591,25 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C27" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E27" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>5</v>
@@ -2629,25 +2623,25 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C28" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E28" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>5</v>
@@ -2661,25 +2655,25 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C29" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E29" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>3</v>
@@ -2693,25 +2687,25 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C30" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E30" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>3</v>
@@ -2725,25 +2719,25 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C31" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E31" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>3</v>
@@ -2757,25 +2751,25 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C32" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E32" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>3</v>
@@ -2789,25 +2783,25 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C33" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E33" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>3</v>
@@ -2821,25 +2815,25 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C34" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E34" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>3</v>
@@ -2853,25 +2847,25 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C35" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E35" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>3</v>
@@ -2885,25 +2879,25 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C36" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E36" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>3</v>
@@ -2917,25 +2911,25 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C37" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C37" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E37" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>3</v>
@@ -2949,25 +2943,25 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C38" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E38" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>3</v>
@@ -2981,25 +2975,25 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C39" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E39" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>3</v>
@@ -3013,25 +3007,25 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C40" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E40" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>13</v>
@@ -3045,25 +3039,25 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C41" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E41" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>13</v>
@@ -3077,25 +3071,25 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C42" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C42" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E42" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>13</v>
@@ -3109,25 +3103,25 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C43" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E43" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>13</v>
@@ -3141,25 +3135,25 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C44" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C44" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E44" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>13</v>
@@ -3173,25 +3167,25 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C45" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C45" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E45" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>13</v>
@@ -3205,25 +3199,25 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C46" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C46" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E46" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>13</v>
@@ -3237,25 +3231,25 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C47" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C47" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E47" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>13</v>
@@ -3269,25 +3263,25 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C48" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D48" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C48" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E48" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>13</v>
@@ -3301,25 +3295,25 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C49" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C49" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E49" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>13</v>
@@ -3333,25 +3327,25 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C50" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C50" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E50" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H50" s="5" t="s">
         <v>13</v>
@@ -3365,25 +3359,25 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C51" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D51" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C51" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E51" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>13</v>
@@ -3397,25 +3391,25 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C52" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C52" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E52" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H52" s="5" t="s">
         <v>15</v>
@@ -3429,25 +3423,25 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C53" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C53" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E53" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>15</v>
@@ -3461,25 +3455,25 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C54" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C54" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E54" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>15</v>
@@ -3493,25 +3487,25 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C55" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D55" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C55" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E55" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>15</v>
@@ -3525,25 +3519,25 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C56" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C56" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E56" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>15</v>
@@ -3557,25 +3551,25 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C57" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D57" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C57" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E57" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H57" s="5" t="s">
         <v>15</v>
@@ -3589,25 +3583,25 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C58" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C58" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E58" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H58" s="5" t="s">
         <v>15</v>
@@ -3621,28 +3615,28 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C59" s="5">
         <v>5905</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>17</v>
@@ -3653,28 +3647,28 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C60" s="5">
         <v>5905</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>17</v>
@@ -3685,28 +3679,28 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C61" s="5">
         <v>5905</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>17</v>
@@ -3717,28 +3711,28 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C62" s="5">
         <v>5905</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>17</v>
@@ -3749,28 +3743,28 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C63" s="5">
         <v>5905</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>17</v>
@@ -3781,28 +3775,28 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C64" s="5">
         <v>5905</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>17</v>
@@ -3813,28 +3807,28 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C65" s="5">
         <v>5905</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>17</v>
@@ -3845,28 +3839,28 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C66" s="5">
         <v>5905</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>17</v>
@@ -3877,28 +3871,28 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C67" s="5">
         <v>5905</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>17</v>
@@ -3909,28 +3903,28 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C68" s="5">
         <v>5905</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>17</v>
@@ -3941,28 +3935,28 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C69" s="5">
         <v>5905</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="I69" s="5" t="s">
         <v>17</v>
@@ -3973,28 +3967,28 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C70" s="5">
         <v>5905</v>
       </c>
       <c r="D70" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F70" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="E70" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>211</v>
-      </c>
       <c r="G70" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="I70" s="5" t="s">
         <v>17</v>
@@ -4005,28 +3999,28 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B71" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C71" s="5">
+        <v>5905</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F71" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C71" s="5">
-        <v>5905</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>212</v>
-      </c>
       <c r="G71" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="I71" s="5" t="s">
         <v>17</v>
@@ -4037,28 +4031,28 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C72" s="5">
         <v>5905</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>17</v>
@@ -4069,28 +4063,28 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C73" s="5">
         <v>5905</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="I73" s="5" t="s">
         <v>17</v>
@@ -4101,28 +4095,28 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C74" s="5">
         <v>5905</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="I74" s="5" t="s">
         <v>17</v>
@@ -4133,28 +4127,28 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C75" s="5">
         <v>5905</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="I75" s="5" t="s">
         <v>17</v>
@@ -4165,28 +4159,28 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C76" s="5">
         <v>5905</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G76" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="H76" s="5" t="s">
         <v>230</v>
-      </c>
-      <c r="H76" s="5" t="s">
-        <v>233</v>
       </c>
       <c r="I76" s="5" t="s">
         <v>17</v>
@@ -4197,28 +4191,28 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C77" s="5">
         <v>5905</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="I77" s="5" t="s">
         <v>17</v>
@@ -4229,28 +4223,28 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C78" s="5">
         <v>5905</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>17</v>
@@ -4261,28 +4255,28 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C79" s="5">
         <v>5905</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>17</v>
@@ -4293,28 +4287,28 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C80" s="5">
         <v>5905</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>17</v>
@@ -4325,28 +4319,28 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C81" s="5">
         <v>5905</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>17</v>
@@ -4357,28 +4351,28 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C82" s="5">
         <v>5905</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>17</v>
@@ -4389,28 +4383,28 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C83" s="5">
         <v>5905</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I83" s="5" t="s">
         <v>17</v>
@@ -4421,28 +4415,28 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C84" s="5">
         <v>5905</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I84" s="5" t="s">
         <v>17</v>
@@ -4453,28 +4447,28 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C85" s="5">
         <v>5905</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I85" s="5" t="s">
         <v>17</v>
@@ -4485,28 +4479,28 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C86" s="5">
         <v>5905</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I86" s="5" t="s">
         <v>17</v>
@@ -4517,28 +4511,28 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C87" s="5">
         <v>5905</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I87" s="5" t="s">
         <v>17</v>
@@ -4549,28 +4543,28 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C88" s="5">
         <v>5905</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G88" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="H88" s="5" t="s">
         <v>256</v>
-      </c>
-      <c r="H88" s="5" t="s">
-        <v>259</v>
       </c>
       <c r="I88" s="5" t="s">
         <v>17</v>
@@ -4581,28 +4575,28 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C89" s="5">
         <v>5905</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H89" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I89" s="5" t="s">
         <v>17</v>
@@ -4613,28 +4607,28 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C90" s="5">
         <v>5905</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H90" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I90" s="5" t="s">
         <v>17</v>
@@ -4645,28 +4639,28 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C91" s="5">
         <v>5905</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="H91" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="I91" s="5" t="s">
         <v>17</v>
@@ -4677,28 +4671,28 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C92" s="5">
         <v>5905</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="H92" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="I92" s="5" t="s">
         <v>17</v>
@@ -4709,28 +4703,28 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C93" s="5">
         <v>5905</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H93" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="I93" s="5" t="s">
         <v>17</v>
@@ -4741,28 +4735,28 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C94" s="5">
         <v>5905</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="H94" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="I94" s="5" t="s">
         <v>17</v>
@@ -4773,28 +4767,28 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C95" s="5">
         <v>5905</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H95" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="I95" s="5" t="s">
         <v>17</v>
@@ -4805,28 +4799,28 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C96" s="5">
         <v>5905</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="H96" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="I96" s="5" t="s">
         <v>17</v>
@@ -4837,28 +4831,28 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C97" s="5">
         <v>5905</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="G97" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="H97" s="5" t="s">
         <v>275</v>
-      </c>
-      <c r="H97" s="5" t="s">
-        <v>278</v>
       </c>
       <c r="I97" s="5" t="s">
         <v>17</v>
@@ -4869,28 +4863,28 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C98" s="5">
         <v>5905</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H98" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="I98" s="5" t="s">
         <v>17</v>
@@ -4901,28 +4895,28 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C99" s="5">
         <v>5905</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H99" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="I99" s="5" t="s">
         <v>17</v>
@@ -4933,25 +4927,25 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C100" s="5">
         <v>5905</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="H100" s="5" t="s">
         <v>13</v>
@@ -4965,25 +4959,25 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C101" s="5">
         <v>5905</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="H101" s="5" t="s">
         <v>13</v>
@@ -4997,25 +4991,25 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C102" s="5">
         <v>5905</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G102" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="H102" s="5" t="s">
         <v>13</v>
@@ -5029,25 +5023,25 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C103" s="5">
         <v>5905</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="H103" s="5" t="s">
         <v>13</v>
@@ -5061,25 +5055,25 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C104" s="5">
         <v>5905</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F104" s="5" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G104" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="H104" s="5" t="s">
         <v>13</v>
@@ -5093,25 +5087,25 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C105" s="5">
         <v>5905</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="H105" s="5" t="s">
         <v>13</v>
@@ -5125,25 +5119,25 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C106" s="5">
         <v>5905</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G106" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="H106" s="5" t="s">
         <v>13</v>
@@ -5157,25 +5151,25 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C107" s="5">
         <v>5905</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G107" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="H107" s="5" t="s">
         <v>13</v>
@@ -5189,25 +5183,25 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C108" s="5">
         <v>5905</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="G108" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="H108" s="5" t="s">
         <v>13</v>
@@ -5221,25 +5215,25 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C109" s="5">
         <v>5905</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G109" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H109" s="5" t="s">
         <v>13</v>
@@ -5253,25 +5247,25 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C110" s="5">
         <v>5905</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G110" s="5" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="H110" s="5" t="s">
         <v>15</v>
@@ -5285,25 +5279,25 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C111" s="5">
         <v>5905</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="H111" s="5" t="s">
         <v>15</v>
@@ -5317,25 +5311,25 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C112" s="5">
         <v>5905</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="H112" s="5" t="s">
         <v>15</v>
@@ -5349,25 +5343,25 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C113" s="5">
         <v>5905</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H113" s="5" t="s">
         <v>15</v>
@@ -5381,25 +5375,25 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C114" s="5">
         <v>5905</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G114" s="5" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H114" s="5" t="s">
         <v>15</v>
@@ -5413,25 +5407,25 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C115" s="5">
         <v>5905</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G115" s="5" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H115" s="5" t="s">
         <v>15</v>
@@ -5445,25 +5439,25 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C116" s="5">
         <v>5905</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="G116" s="5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="H116" s="5" t="s">
         <v>15</v>
@@ -5477,25 +5471,25 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C117" s="5">
         <v>5905</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G117" s="5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="H117" s="5" t="s">
         <v>15</v>
@@ -5509,25 +5503,25 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C118" s="5">
         <v>5905</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F118" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G118" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="H118" s="5" t="s">
         <v>15</v>
@@ -5541,25 +5535,25 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C119" s="5">
         <v>5905</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G119" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H119" s="5" t="s">
         <v>15</v>
@@ -5573,25 +5567,25 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>209</v>
+        <v>318</v>
       </c>
       <c r="C120" s="5">
         <v>5905</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="G120" s="5" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="H120" s="5" t="s">
         <v>15</v>
@@ -5611,7 +5605,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5669,7 +5663,7 @@
         <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
         <v>54</v>

</xml_diff>